<commit_message>
pd_dinh: update lyaout again
</commit_message>
<xml_diff>
--- a/data/DATA.xlsx
+++ b/data/DATA.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="2026" sheetId="1" r:id="rId1"/>
@@ -1090,7 +1090,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1412,7 +1412,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1854,7 +1854,7 @@
         <v>133</v>
       </c>
       <c r="G19" t="s">
-        <v>70</v>
+        <v>227</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -2504,7 +2504,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:G11 B22:G30 A14:G21 A12:E12 G12 A13 B32:G47" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:G11 B22:G30 A14:G18 A12:E12 G12 A13 B32:G47 A20:G21 A19:F19" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix render year and add data
</commit_message>
<xml_diff>
--- a/data/DATA.xlsx
+++ b/data/DATA.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pd_dinh\Desktop\CODE_CT\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\01_LY THANH TUNG\04_LEARN\01_CODE\01_GIT\04_CHANH_TAM\hoc-chung-chanh-tam\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="234">
   <si>
     <t>id</t>
   </si>
@@ -232,9 +232,6 @@
     <t>Nhật Uyên xinh đẹp</t>
   </si>
   <si>
-    <t>./images/USER.png</t>
-  </si>
-  <si>
     <t>Lý Thanh Tùng (Tbh)</t>
   </si>
   <si>
@@ -304,9 +301,6 @@
     <t>Trưởng ban hậu cần</t>
   </si>
   <si>
-    <t>Má hồng</t>
-  </si>
-  <si>
     <t>./images/NGUYEN_THI_HUYNH_THANH.jpg</t>
   </si>
   <si>
@@ -421,9 +415,6 @@
     <t>Nhã</t>
   </si>
   <si>
-    <t>Tôm Nhõ</t>
-  </si>
-  <si>
     <t>19</t>
   </si>
   <si>
@@ -704,13 +695,34 @@
   </si>
   <si>
     <t>./images/HUYNH_NGUYEN_TAM_NHA.jpg</t>
-  </si>
-  <si>
-    <t>…</t>
   </si>
   <si>
     <t xml:space="preserve">./images/NGUYEN_DANG_HUY.jpg
 </t>
+  </si>
+  <si>
+    <t>Lớp trưởng 2019-2023</t>
+  </si>
+  <si>
+    <t>./images/NGUYEN_NGOC_KY_DUYEN.jpg</t>
+  </si>
+  <si>
+    <t>Má hồng 😳</t>
+  </si>
+  <si>
+    <t>Bộ trưởng bộ ngoại giao</t>
+  </si>
+  <si>
+    <t>🍓</t>
+  </si>
+  <si>
+    <t>Hồ Tâm Nguyên</t>
+  </si>
+  <si>
+    <t>Nguyên</t>
+  </si>
+  <si>
+    <t>Trưởng ban truyền thông 2022-2024</t>
   </si>
 </sst>
 </file>
@@ -1088,20 +1100,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="2" max="2" width="30.375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.5" customWidth="1"/>
     <col min="4" max="4" width="21.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.75" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="39" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="39" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1124,107 +1138,107 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>107</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>104</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>180</v>
       </c>
       <c r="E2" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="F2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>105</v>
+        <v>178</v>
       </c>
       <c r="C3" t="s">
-        <v>106</v>
+        <v>179</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>180</v>
       </c>
       <c r="E3" t="s">
         <v>40</v>
       </c>
       <c r="F3" t="s">
-        <v>226</v>
+        <v>181</v>
       </c>
       <c r="G3" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="F4" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="G4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>103</v>
       </c>
       <c r="C5" t="s">
-        <v>23</v>
+        <v>104</v>
       </c>
       <c r="D5" t="s">
         <v>17</v>
       </c>
       <c r="E5" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="F5" t="s">
-        <v>25</v>
+        <v>223</v>
       </c>
       <c r="G5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="D6" t="s">
         <v>17</v>
@@ -1233,67 +1247,67 @@
         <v>18</v>
       </c>
       <c r="F6" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="G6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>33</v>
+        <v>85</v>
       </c>
       <c r="C7" t="s">
-        <v>34</v>
+        <v>86</v>
       </c>
       <c r="D7" t="s">
-        <v>17</v>
+        <v>87</v>
       </c>
       <c r="E7" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="F7" t="s">
-        <v>35</v>
+        <v>88</v>
       </c>
       <c r="G7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="C8" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="D8" t="s">
         <v>17</v>
       </c>
       <c r="E8" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="F8" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="G8" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="C9" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="D9" t="s">
         <v>17</v>
@@ -1302,125 +1316,245 @@
         <v>18</v>
       </c>
       <c r="F9" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="G9" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="C10" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="D10" t="s">
         <v>17</v>
       </c>
       <c r="E10" t="s">
-        <v>51</v>
+        <v>24</v>
       </c>
       <c r="F10" t="s">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="G10" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="C11" t="s">
-        <v>56</v>
+        <v>39</v>
       </c>
       <c r="D11" t="s">
         <v>17</v>
       </c>
       <c r="E11" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="F11" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="G11" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="C12" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="D12" t="s">
-        <v>62</v>
+        <v>17</v>
       </c>
       <c r="E12" t="s">
-        <v>63</v>
+        <v>18</v>
       </c>
       <c r="F12" t="s">
-        <v>64</v>
+        <v>46</v>
       </c>
       <c r="G12" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>131</v>
+        <v>49</v>
       </c>
       <c r="C13" t="s">
-        <v>132</v>
+        <v>50</v>
       </c>
       <c r="D13" t="s">
         <v>17</v>
       </c>
       <c r="E13" t="s">
+        <v>51</v>
+      </c>
+      <c r="F13" t="s">
+        <v>52</v>
+      </c>
+      <c r="G13" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>55</v>
+      </c>
+      <c r="C14" t="s">
+        <v>56</v>
+      </c>
+      <c r="D14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" t="s">
+        <v>57</v>
+      </c>
+      <c r="G14" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>129</v>
+      </c>
+      <c r="C15" t="s">
+        <v>130</v>
+      </c>
+      <c r="D15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" t="s">
         <v>24</v>
       </c>
-      <c r="F13" t="s">
-        <v>228</v>
-      </c>
-      <c r="G13" t="s">
+      <c r="F15" t="s">
+        <v>229</v>
+      </c>
+      <c r="G15" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>94</v>
+      </c>
+      <c r="C16" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" t="s">
+        <v>180</v>
+      </c>
+      <c r="E16" t="s">
+        <v>63</v>
+      </c>
+      <c r="F16" t="s">
+        <v>96</v>
+      </c>
+      <c r="G16" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>170</v>
+      </c>
+      <c r="C17" t="s">
+        <v>140</v>
+      </c>
+      <c r="D17" t="s">
+        <v>180</v>
+      </c>
+      <c r="E17" t="s">
+        <v>51</v>
+      </c>
+      <c r="F17" t="s">
+        <v>230</v>
+      </c>
+      <c r="G17" t="s">
         <v>227</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A18">
+        <v>18</v>
+      </c>
+      <c r="B18" t="s">
+        <v>60</v>
+      </c>
+      <c r="C18" t="s">
+        <v>61</v>
+      </c>
+      <c r="D18" t="s">
+        <v>62</v>
+      </c>
+      <c r="E18" t="s">
+        <v>63</v>
+      </c>
+      <c r="F18" t="s">
+        <v>64</v>
+      </c>
+      <c r="G18" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="B4:G12 A1:G1 B2:G2" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:G1" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G47"/>
+  <dimension ref="A1:G48"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7:G7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="2" max="2" width="30.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="41.8125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="31" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="39" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1443,7 +1577,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1462,34 +1596,31 @@
       <c r="F2" t="s">
         <v>69</v>
       </c>
-      <c r="G2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>14</v>
       </c>
       <c r="B3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3" t="s">
         <v>71</v>
-      </c>
-      <c r="C3" t="s">
-        <v>72</v>
       </c>
       <c r="D3" t="s">
         <v>67</v>
       </c>
       <c r="E3" t="s">
+        <v>72</v>
+      </c>
+      <c r="F3" t="s">
         <v>73</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>74</v>
       </c>
-      <c r="G3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -1512,122 +1643,122 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
         <v>27</v>
       </c>
       <c r="B5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C5" t="s">
         <v>76</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>77</v>
-      </c>
-      <c r="D5" t="s">
-        <v>78</v>
       </c>
       <c r="E5" t="s">
         <v>51</v>
       </c>
       <c r="F5" t="s">
+        <v>78</v>
+      </c>
+      <c r="G5" t="s">
         <v>79</v>
       </c>
-      <c r="G5" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
         <v>32</v>
       </c>
       <c r="B6" t="s">
+        <v>80</v>
+      </c>
+      <c r="C6" t="s">
         <v>81</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>82</v>
-      </c>
-      <c r="D6" t="s">
-        <v>83</v>
       </c>
       <c r="E6" t="s">
         <v>11</v>
       </c>
       <c r="F6" t="s">
+        <v>83</v>
+      </c>
+      <c r="G6" t="s">
         <v>84</v>
       </c>
-      <c r="G6" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
         <v>37</v>
       </c>
       <c r="B7" t="s">
+        <v>85</v>
+      </c>
+      <c r="C7" t="s">
         <v>86</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>87</v>
-      </c>
-      <c r="D7" t="s">
-        <v>88</v>
       </c>
       <c r="E7" t="s">
         <v>40</v>
       </c>
       <c r="F7" t="s">
+        <v>88</v>
+      </c>
+      <c r="G7" t="s">
         <v>89</v>
       </c>
-      <c r="G7" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
         <v>43</v>
       </c>
       <c r="B8" t="s">
+        <v>90</v>
+      </c>
+      <c r="C8" t="s">
         <v>91</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>92</v>
-      </c>
-      <c r="D8" t="s">
-        <v>93</v>
       </c>
       <c r="E8" t="s">
         <v>11</v>
       </c>
       <c r="F8" t="s">
-        <v>94</v>
+        <v>228</v>
       </c>
       <c r="G8" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
         <v>48</v>
       </c>
       <c r="B9" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C9" t="s">
         <v>39</v>
       </c>
       <c r="D9" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E9" t="s">
         <v>63</v>
       </c>
       <c r="F9" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G9" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
         <v>54</v>
       </c>
@@ -1650,15 +1781,15 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A11" t="s">
         <v>59</v>
       </c>
       <c r="B11" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C11" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D11" t="s">
         <v>17</v>
@@ -1667,21 +1798,21 @@
         <v>11</v>
       </c>
       <c r="F11" t="s">
+        <v>100</v>
+      </c>
+      <c r="G11" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A12" t="s">
         <v>102</v>
       </c>
-      <c r="G11" t="s">
+      <c r="B12" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="C12" t="s">
         <v>104</v>
-      </c>
-      <c r="B12" t="s">
-        <v>105</v>
-      </c>
-      <c r="C12" t="s">
-        <v>106</v>
       </c>
       <c r="D12" t="s">
         <v>17</v>
@@ -1690,44 +1821,41 @@
         <v>40</v>
       </c>
       <c r="F12" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="G12" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A13" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B13" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C13" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="D13" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="E13" t="s">
         <v>51</v>
       </c>
       <c r="F13" t="s">
-        <v>179</v>
-      </c>
-      <c r="G13" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A14" t="s">
+        <v>109</v>
+      </c>
+      <c r="B14" t="s">
+        <v>110</v>
+      </c>
+      <c r="C14" t="s">
         <v>111</v>
-      </c>
-      <c r="B14" t="s">
-        <v>112</v>
-      </c>
-      <c r="C14" t="s">
-        <v>113</v>
       </c>
       <c r="D14" t="s">
         <v>17</v>
@@ -1736,18 +1864,15 @@
         <v>63</v>
       </c>
       <c r="F14" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A15" t="s">
+        <v>113</v>
+      </c>
+      <c r="B15" t="s">
         <v>114</v>
-      </c>
-      <c r="G14" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>115</v>
-      </c>
-      <c r="B15" t="s">
-        <v>116</v>
       </c>
       <c r="C15" t="s">
         <v>16</v>
@@ -1759,21 +1884,18 @@
         <v>40</v>
       </c>
       <c r="F15" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A16" t="s">
+        <v>116</v>
+      </c>
+      <c r="B16" t="s">
         <v>117</v>
       </c>
-      <c r="G15" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="C16" t="s">
         <v>118</v>
-      </c>
-      <c r="B16" t="s">
-        <v>119</v>
-      </c>
-      <c r="C16" t="s">
-        <v>120</v>
       </c>
       <c r="D16" t="s">
         <v>17</v>
@@ -1782,21 +1904,18 @@
         <v>40</v>
       </c>
       <c r="F16" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A17" t="s">
+        <v>120</v>
+      </c>
+      <c r="B17" t="s">
         <v>121</v>
       </c>
-      <c r="G16" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="C17" t="s">
         <v>122</v>
-      </c>
-      <c r="B17" t="s">
-        <v>123</v>
-      </c>
-      <c r="C17" t="s">
-        <v>124</v>
       </c>
       <c r="D17" t="s">
         <v>17</v>
@@ -1805,21 +1924,18 @@
         <v>11</v>
       </c>
       <c r="F17" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A18" t="s">
+        <v>124</v>
+      </c>
+      <c r="B18" t="s">
         <v>125</v>
       </c>
-      <c r="G17" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="C18" t="s">
         <v>126</v>
-      </c>
-      <c r="B18" t="s">
-        <v>127</v>
-      </c>
-      <c r="C18" t="s">
-        <v>128</v>
       </c>
       <c r="D18" t="s">
         <v>17</v>
@@ -1828,21 +1944,18 @@
         <v>51</v>
       </c>
       <c r="F18" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A19" t="s">
+        <v>128</v>
+      </c>
+      <c r="B19" t="s">
         <v>129</v>
       </c>
-      <c r="G18" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="C19" t="s">
         <v>130</v>
-      </c>
-      <c r="B19" t="s">
-        <v>131</v>
-      </c>
-      <c r="C19" t="s">
-        <v>132</v>
       </c>
       <c r="D19" t="s">
         <v>17</v>
@@ -1851,21 +1964,21 @@
         <v>24</v>
       </c>
       <c r="F19" t="s">
+        <v>229</v>
+      </c>
+      <c r="G19" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A20" t="s">
+        <v>131</v>
+      </c>
+      <c r="B20" t="s">
+        <v>132</v>
+      </c>
+      <c r="C20" t="s">
         <v>133</v>
-      </c>
-      <c r="G19" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>134</v>
-      </c>
-      <c r="B20" t="s">
-        <v>135</v>
-      </c>
-      <c r="C20" t="s">
-        <v>136</v>
       </c>
       <c r="D20" t="s">
         <v>17</v>
@@ -1874,18 +1987,15 @@
         <v>11</v>
       </c>
       <c r="F20" t="s">
-        <v>137</v>
-      </c>
-      <c r="G20" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A21" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B21" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C21" t="s">
         <v>23</v>
@@ -1897,21 +2007,18 @@
         <v>24</v>
       </c>
       <c r="F21" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A22" t="s">
+        <v>138</v>
+      </c>
+      <c r="B22" t="s">
+        <v>139</v>
+      </c>
+      <c r="C22" t="s">
         <v>140</v>
-      </c>
-      <c r="G21" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>141</v>
-      </c>
-      <c r="B22" t="s">
-        <v>142</v>
-      </c>
-      <c r="C22" t="s">
-        <v>143</v>
       </c>
       <c r="D22" t="s">
         <v>17</v>
@@ -1920,21 +2027,18 @@
         <v>40</v>
       </c>
       <c r="F22" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A23" t="s">
+        <v>142</v>
+      </c>
+      <c r="B23" t="s">
+        <v>143</v>
+      </c>
+      <c r="C23" t="s">
         <v>144</v>
-      </c>
-      <c r="G22" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>145</v>
-      </c>
-      <c r="B23" t="s">
-        <v>146</v>
-      </c>
-      <c r="C23" t="s">
-        <v>147</v>
       </c>
       <c r="D23" t="s">
         <v>17</v>
@@ -1943,18 +2047,15 @@
         <v>40</v>
       </c>
       <c r="F23" t="s">
-        <v>148</v>
-      </c>
-      <c r="G23" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A24" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B24" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C24" t="s">
         <v>39</v>
@@ -1966,21 +2067,18 @@
         <v>18</v>
       </c>
       <c r="F24" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A25" t="s">
+        <v>149</v>
+      </c>
+      <c r="B25" t="s">
+        <v>150</v>
+      </c>
+      <c r="C25" t="s">
         <v>151</v>
-      </c>
-      <c r="G24" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>152</v>
-      </c>
-      <c r="B25" t="s">
-        <v>153</v>
-      </c>
-      <c r="C25" t="s">
-        <v>154</v>
       </c>
       <c r="D25" t="s">
         <v>17</v>
@@ -1989,21 +2087,18 @@
         <v>18</v>
       </c>
       <c r="F25" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A26" t="s">
+        <v>153</v>
+      </c>
+      <c r="B26" t="s">
+        <v>154</v>
+      </c>
+      <c r="C26" t="s">
         <v>155</v>
-      </c>
-      <c r="G25" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>156</v>
-      </c>
-      <c r="B26" t="s">
-        <v>157</v>
-      </c>
-      <c r="C26" t="s">
-        <v>158</v>
       </c>
       <c r="D26" t="s">
         <v>17</v>
@@ -2012,21 +2107,18 @@
         <v>63</v>
       </c>
       <c r="F26" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A27" t="s">
+        <v>157</v>
+      </c>
+      <c r="B27" t="s">
+        <v>158</v>
+      </c>
+      <c r="C27" t="s">
         <v>159</v>
-      </c>
-      <c r="G26" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>160</v>
-      </c>
-      <c r="B27" t="s">
-        <v>161</v>
-      </c>
-      <c r="C27" t="s">
-        <v>162</v>
       </c>
       <c r="D27" t="s">
         <v>17</v>
@@ -2035,21 +2127,21 @@
         <v>63</v>
       </c>
       <c r="F27" t="s">
+        <v>160</v>
+      </c>
+      <c r="G27" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A28" t="s">
+        <v>162</v>
+      </c>
+      <c r="B28" t="s">
         <v>163</v>
       </c>
-      <c r="G27" t="s">
+      <c r="C28" t="s">
         <v>164</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>165</v>
-      </c>
-      <c r="B28" t="s">
-        <v>166</v>
-      </c>
-      <c r="C28" t="s">
-        <v>167</v>
       </c>
       <c r="D28" t="s">
         <v>17</v>
@@ -2058,18 +2150,15 @@
         <v>63</v>
       </c>
       <c r="F28" t="s">
-        <v>168</v>
-      </c>
-      <c r="G28" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A29" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B29" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C29" t="s">
         <v>23</v>
@@ -2081,21 +2170,18 @@
         <v>51</v>
       </c>
       <c r="F29" t="s">
-        <v>171</v>
-      </c>
-      <c r="G29" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A30" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B30" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C30" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="D30" t="s">
         <v>17</v>
@@ -2104,21 +2190,21 @@
         <v>51</v>
       </c>
       <c r="F30" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="G30" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A31" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B31" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C31" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D31" t="s">
         <v>17</v>
@@ -2127,156 +2213,147 @@
         <v>24</v>
       </c>
       <c r="F31" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A32" t="s">
+        <v>177</v>
+      </c>
+      <c r="B32" t="s">
+        <v>178</v>
+      </c>
+      <c r="C32" t="s">
+        <v>179</v>
+      </c>
+      <c r="D32" t="s">
         <v>180</v>
-      </c>
-      <c r="B32" t="s">
-        <v>181</v>
-      </c>
-      <c r="C32" t="s">
-        <v>182</v>
-      </c>
-      <c r="D32" t="s">
-        <v>183</v>
       </c>
       <c r="E32" t="s">
         <v>40</v>
       </c>
       <c r="F32" t="s">
+        <v>181</v>
+      </c>
+      <c r="G32" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A33" t="s">
+        <v>183</v>
+      </c>
+      <c r="B33" t="s">
         <v>184</v>
       </c>
-      <c r="G32" t="s">
+      <c r="C33" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>186</v>
-      </c>
-      <c r="B33" t="s">
-        <v>187</v>
-      </c>
-      <c r="C33" t="s">
-        <v>188</v>
-      </c>
       <c r="D33" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="E33" t="s">
         <v>24</v>
       </c>
       <c r="F33" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A34" t="s">
+        <v>187</v>
+      </c>
+      <c r="B34" t="s">
+        <v>188</v>
+      </c>
+      <c r="C34" t="s">
         <v>189</v>
       </c>
-      <c r="G33" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="D34" t="s">
+        <v>180</v>
+      </c>
+      <c r="E34" t="s">
         <v>190</v>
       </c>
-      <c r="B34" t="s">
+      <c r="F34" t="s">
         <v>191</v>
       </c>
-      <c r="C34" t="s">
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A35" t="s">
         <v>192</v>
       </c>
-      <c r="D34" t="s">
-        <v>183</v>
-      </c>
-      <c r="E34" t="s">
+      <c r="B35" t="s">
         <v>193</v>
       </c>
-      <c r="F34" t="s">
+      <c r="C35" t="s">
         <v>194</v>
       </c>
-      <c r="G34" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>195</v>
-      </c>
-      <c r="B35" t="s">
-        <v>196</v>
-      </c>
-      <c r="C35" t="s">
-        <v>197</v>
-      </c>
       <c r="D35" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="E35" t="s">
         <v>51</v>
       </c>
       <c r="F35" t="s">
+        <v>195</v>
+      </c>
+      <c r="G35" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A36" t="s">
+        <v>197</v>
+      </c>
+      <c r="B36" t="s">
         <v>198</v>
       </c>
-      <c r="G35" t="s">
+      <c r="C36" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>200</v>
-      </c>
-      <c r="B36" t="s">
-        <v>201</v>
-      </c>
-      <c r="C36" t="s">
-        <v>202</v>
-      </c>
       <c r="D36" t="s">
-        <v>183</v>
+        <v>226</v>
       </c>
       <c r="E36" t="s">
         <v>63</v>
       </c>
       <c r="F36" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A37" t="s">
+        <v>201</v>
+      </c>
+      <c r="B37" t="s">
+        <v>202</v>
+      </c>
+      <c r="C37" t="s">
         <v>203</v>
       </c>
-      <c r="G36" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>204</v>
-      </c>
-      <c r="B37" t="s">
-        <v>205</v>
-      </c>
-      <c r="C37" t="s">
-        <v>206</v>
-      </c>
       <c r="D37" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="E37" t="s">
         <v>18</v>
       </c>
       <c r="F37" t="s">
+        <v>204</v>
+      </c>
+      <c r="G37" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A38" t="s">
+        <v>206</v>
+      </c>
+      <c r="B38" t="s">
         <v>207</v>
-      </c>
-      <c r="G37" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>209</v>
-      </c>
-      <c r="B38" t="s">
-        <v>210</v>
       </c>
       <c r="C38" t="s">
         <v>23</v>
@@ -2288,15 +2365,15 @@
         <v>24</v>
       </c>
       <c r="F38" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G38" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A39" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="B39" t="s">
         <v>33</v>
@@ -2317,9 +2394,9 @@
         <v>36</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A40" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B40" t="s">
         <v>60</v>
@@ -2340,9 +2417,9 @@
         <v>65</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A41" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B41" t="s">
         <v>22</v>
@@ -2363,9 +2440,9 @@
         <v>26</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A42" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B42" t="s">
         <v>28</v>
@@ -2386,9 +2463,9 @@
         <v>31</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A43" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B43" t="s">
         <v>33</v>
@@ -2406,12 +2483,12 @@
         <v>35</v>
       </c>
       <c r="G43" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A44" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B44" t="s">
         <v>38</v>
@@ -2429,12 +2506,12 @@
         <v>41</v>
       </c>
       <c r="G44" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A45" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B45" t="s">
         <v>44</v>
@@ -2452,12 +2529,12 @@
         <v>46</v>
       </c>
       <c r="G45" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A46" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B46" t="s">
         <v>49</v>
@@ -2475,12 +2552,12 @@
         <v>52</v>
       </c>
       <c r="G46" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A47" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B47" t="s">
         <v>55</v>
@@ -2499,12 +2576,26 @@
       </c>
       <c r="G47" t="s">
         <v>58</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="B48" t="s">
+        <v>231</v>
+      </c>
+      <c r="C48" t="s">
+        <v>232</v>
+      </c>
+      <c r="D48" t="s">
+        <v>233</v>
+      </c>
+      <c r="E48" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:G11 B22:G30 A14:G18 A12:E12 G12 A13 B32:G47 A20:G21 A19:F19" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:G1 B27:G27 A14:F18 A12:E12 G12 A13 B32:G32 A20:F21 A19:E19 B37:G47 B36:C36 E36:F36 B30:F30 A9:G11 A8:E8 G8 B35:G35 B34:F34 B33:F33 B22:F26 A3:G7 A2:F2 B28:F29" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix show default image
</commit_message>
<xml_diff>
--- a/data/DATA.xlsx
+++ b/data/DATA.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="236">
   <si>
     <t>id</t>
   </si>
@@ -723,6 +723,12 @@
   </si>
   <si>
     <t>Trưởng ban truyền thông 2022-2024</t>
+  </si>
+  <si>
+    <t>Chú rể Huy</t>
+  </si>
+  <si>
+    <t>Cô dâu Chi</t>
   </si>
 </sst>
 </file>
@@ -1103,7 +1109,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -1155,7 +1161,7 @@
         <v>24</v>
       </c>
       <c r="F2" t="s">
-        <v>108</v>
+        <v>234</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>225</v>
@@ -1178,7 +1184,7 @@
         <v>40</v>
       </c>
       <c r="F3" t="s">
-        <v>181</v>
+        <v>235</v>
       </c>
       <c r="G3" t="s">
         <v>182</v>

</xml_diff>

<commit_message>
fix logo and edit data
</commit_message>
<xml_diff>
--- a/data/DATA.xlsx
+++ b/data/DATA.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="2026" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="236">
   <si>
     <t>id</t>
   </si>
@@ -331,9 +331,6 @@
     <t>11</t>
   </si>
   <si>
-    <t>Lê Văn Huy</t>
-  </si>
-  <si>
     <t>Huy</t>
   </si>
   <si>
@@ -665,9 +662,6 @@
   </si>
   <si>
     <t>42</t>
-  </si>
-  <si>
-    <t>./images/TRAN_THI_XUAN_DIEU.jpg_x000D_</t>
   </si>
   <si>
     <t>43</t>
@@ -716,9 +710,6 @@
     <t>🍓</t>
   </si>
   <si>
-    <t>Hồ Tâm Nguyên</t>
-  </si>
-  <si>
     <t>Nguyên</t>
   </si>
   <si>
@@ -729,6 +720,15 @@
   </si>
   <si>
     <t>Cô dâu Chi</t>
+  </si>
+  <si>
+    <t>Hồ Tâm Nguyên (Nguyên Hồ)</t>
+  </si>
+  <si>
+    <t>Lê Văn Huy (Huy Lê)</t>
+  </si>
+  <si>
+    <t>Sâu sắc</t>
   </si>
 </sst>
 </file>
@@ -1108,8 +1108,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -1149,22 +1149,22 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E2" t="s">
         <v>24</v>
       </c>
       <c r="F2" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.5">
@@ -1172,22 +1172,22 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>177</v>
+      </c>
+      <c r="C3" t="s">
         <v>178</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>179</v>
-      </c>
-      <c r="D3" t="s">
-        <v>180</v>
       </c>
       <c r="E3" t="s">
         <v>40</v>
       </c>
       <c r="F3" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="G3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.5">
@@ -1218,10 +1218,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>234</v>
+      </c>
+      <c r="C5" t="s">
         <v>103</v>
-      </c>
-      <c r="C5" t="s">
-        <v>104</v>
       </c>
       <c r="D5" t="s">
         <v>17</v>
@@ -1230,10 +1230,10 @@
         <v>40</v>
       </c>
       <c r="F5" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="G5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.5">
@@ -1448,10 +1448,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
+        <v>128</v>
+      </c>
+      <c r="C15" t="s">
         <v>129</v>
-      </c>
-      <c r="C15" t="s">
-        <v>130</v>
       </c>
       <c r="D15" t="s">
         <v>17</v>
@@ -1460,10 +1460,10 @@
         <v>24</v>
       </c>
       <c r="F15" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="G15" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.5">
@@ -1477,7 +1477,7 @@
         <v>39</v>
       </c>
       <c r="D16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E16" t="s">
         <v>63</v>
@@ -1494,22 +1494,22 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C17" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D17" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E17" t="s">
         <v>51</v>
       </c>
       <c r="F17" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="G17" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.5">
@@ -1545,10 +1545,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G48"/>
+  <dimension ref="A1:G47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:G7"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="F48" sqref="F48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -1735,7 +1735,7 @@
         <v>11</v>
       </c>
       <c r="F8" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="G8" t="s">
         <v>93</v>
@@ -1815,10 +1815,10 @@
         <v>102</v>
       </c>
       <c r="B12" t="s">
+        <v>234</v>
+      </c>
+      <c r="C12" t="s">
         <v>103</v>
-      </c>
-      <c r="C12" t="s">
-        <v>104</v>
       </c>
       <c r="D12" t="s">
         <v>17</v>
@@ -1827,41 +1827,41 @@
         <v>40</v>
       </c>
       <c r="F12" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="G12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B13" t="s">
+        <v>172</v>
+      </c>
+      <c r="C13" t="s">
         <v>173</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>174</v>
-      </c>
-      <c r="D13" t="s">
-        <v>175</v>
       </c>
       <c r="E13" t="s">
         <v>51</v>
       </c>
       <c r="F13" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A14" t="s">
+        <v>108</v>
+      </c>
+      <c r="B14" t="s">
         <v>109</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>110</v>
-      </c>
-      <c r="C14" t="s">
-        <v>111</v>
       </c>
       <c r="D14" t="s">
         <v>17</v>
@@ -1870,15 +1870,15 @@
         <v>63</v>
       </c>
       <c r="F14" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A15" t="s">
+        <v>112</v>
+      </c>
+      <c r="B15" t="s">
         <v>113</v>
-      </c>
-      <c r="B15" t="s">
-        <v>114</v>
       </c>
       <c r="C15" t="s">
         <v>16</v>
@@ -1890,18 +1890,18 @@
         <v>40</v>
       </c>
       <c r="F15" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A16" t="s">
+        <v>115</v>
+      </c>
+      <c r="B16" t="s">
         <v>116</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>117</v>
-      </c>
-      <c r="C16" t="s">
-        <v>118</v>
       </c>
       <c r="D16" t="s">
         <v>17</v>
@@ -1910,18 +1910,18 @@
         <v>40</v>
       </c>
       <c r="F16" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A17" t="s">
+        <v>119</v>
+      </c>
+      <c r="B17" t="s">
         <v>120</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>121</v>
-      </c>
-      <c r="C17" t="s">
-        <v>122</v>
       </c>
       <c r="D17" t="s">
         <v>17</v>
@@ -1930,18 +1930,18 @@
         <v>11</v>
       </c>
       <c r="F17" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A18" t="s">
+        <v>123</v>
+      </c>
+      <c r="B18" t="s">
         <v>124</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>125</v>
-      </c>
-      <c r="C18" t="s">
-        <v>126</v>
       </c>
       <c r="D18" t="s">
         <v>17</v>
@@ -1950,18 +1950,18 @@
         <v>51</v>
       </c>
       <c r="F18" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A19" t="s">
+        <v>127</v>
+      </c>
+      <c r="B19" t="s">
         <v>128</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>129</v>
-      </c>
-      <c r="C19" t="s">
-        <v>130</v>
       </c>
       <c r="D19" t="s">
         <v>17</v>
@@ -1970,21 +1970,21 @@
         <v>24</v>
       </c>
       <c r="F19" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="G19" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A20" t="s">
+        <v>130</v>
+      </c>
+      <c r="B20" t="s">
         <v>131</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>132</v>
-      </c>
-      <c r="C20" t="s">
-        <v>133</v>
       </c>
       <c r="D20" t="s">
         <v>17</v>
@@ -1993,15 +1993,15 @@
         <v>11</v>
       </c>
       <c r="F20" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A21" t="s">
+        <v>134</v>
+      </c>
+      <c r="B21" t="s">
         <v>135</v>
-      </c>
-      <c r="B21" t="s">
-        <v>136</v>
       </c>
       <c r="C21" t="s">
         <v>23</v>
@@ -2013,18 +2013,18 @@
         <v>24</v>
       </c>
       <c r="F21" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A22" t="s">
+        <v>137</v>
+      </c>
+      <c r="B22" t="s">
         <v>138</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>139</v>
-      </c>
-      <c r="C22" t="s">
-        <v>140</v>
       </c>
       <c r="D22" t="s">
         <v>17</v>
@@ -2033,18 +2033,18 @@
         <v>40</v>
       </c>
       <c r="F22" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A23" t="s">
+        <v>141</v>
+      </c>
+      <c r="B23" t="s">
         <v>142</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
         <v>143</v>
-      </c>
-      <c r="C23" t="s">
-        <v>144</v>
       </c>
       <c r="D23" t="s">
         <v>17</v>
@@ -2053,15 +2053,15 @@
         <v>40</v>
       </c>
       <c r="F23" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A24" t="s">
+        <v>145</v>
+      </c>
+      <c r="B24" t="s">
         <v>146</v>
-      </c>
-      <c r="B24" t="s">
-        <v>147</v>
       </c>
       <c r="C24" t="s">
         <v>39</v>
@@ -2073,18 +2073,18 @@
         <v>18</v>
       </c>
       <c r="F24" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A25" t="s">
+        <v>148</v>
+      </c>
+      <c r="B25" t="s">
         <v>149</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" t="s">
         <v>150</v>
-      </c>
-      <c r="C25" t="s">
-        <v>151</v>
       </c>
       <c r="D25" t="s">
         <v>17</v>
@@ -2093,18 +2093,18 @@
         <v>18</v>
       </c>
       <c r="F25" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A26" t="s">
+        <v>152</v>
+      </c>
+      <c r="B26" t="s">
         <v>153</v>
       </c>
-      <c r="B26" t="s">
+      <c r="C26" t="s">
         <v>154</v>
-      </c>
-      <c r="C26" t="s">
-        <v>155</v>
       </c>
       <c r="D26" t="s">
         <v>17</v>
@@ -2113,18 +2113,18 @@
         <v>63</v>
       </c>
       <c r="F26" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A27" t="s">
+        <v>156</v>
+      </c>
+      <c r="B27" t="s">
         <v>157</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
         <v>158</v>
-      </c>
-      <c r="C27" t="s">
-        <v>159</v>
       </c>
       <c r="D27" t="s">
         <v>17</v>
@@ -2133,21 +2133,21 @@
         <v>63</v>
       </c>
       <c r="F27" t="s">
+        <v>159</v>
+      </c>
+      <c r="G27" t="s">
         <v>160</v>
-      </c>
-      <c r="G27" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A28" t="s">
+        <v>161</v>
+      </c>
+      <c r="B28" t="s">
         <v>162</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" t="s">
         <v>163</v>
-      </c>
-      <c r="C28" t="s">
-        <v>164</v>
       </c>
       <c r="D28" t="s">
         <v>17</v>
@@ -2156,15 +2156,15 @@
         <v>63</v>
       </c>
       <c r="F28" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A29" t="s">
+        <v>165</v>
+      </c>
+      <c r="B29" t="s">
         <v>166</v>
-      </c>
-      <c r="B29" t="s">
-        <v>167</v>
       </c>
       <c r="C29" t="s">
         <v>23</v>
@@ -2176,18 +2176,18 @@
         <v>51</v>
       </c>
       <c r="F29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A30" t="s">
+        <v>168</v>
+      </c>
+      <c r="B30" t="s">
         <v>169</v>
       </c>
-      <c r="B30" t="s">
-        <v>170</v>
-      </c>
       <c r="C30" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D30" t="s">
         <v>17</v>
@@ -2196,21 +2196,21 @@
         <v>51</v>
       </c>
       <c r="F30" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G30" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A31" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B31" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C31" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D31" t="s">
         <v>17</v>
@@ -2219,147 +2219,147 @@
         <v>24</v>
       </c>
       <c r="F31" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A32" t="s">
+        <v>176</v>
+      </c>
+      <c r="B32" t="s">
         <v>177</v>
       </c>
-      <c r="B32" t="s">
+      <c r="C32" t="s">
         <v>178</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D32" t="s">
         <v>179</v>
-      </c>
-      <c r="D32" t="s">
-        <v>180</v>
       </c>
       <c r="E32" t="s">
         <v>40</v>
       </c>
       <c r="F32" t="s">
+        <v>180</v>
+      </c>
+      <c r="G32" t="s">
         <v>181</v>
-      </c>
-      <c r="G32" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A33" t="s">
+        <v>182</v>
+      </c>
+      <c r="B33" t="s">
         <v>183</v>
       </c>
-      <c r="B33" t="s">
+      <c r="C33" t="s">
         <v>184</v>
       </c>
-      <c r="C33" t="s">
-        <v>185</v>
-      </c>
       <c r="D33" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E33" t="s">
         <v>24</v>
       </c>
       <c r="F33" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A34" t="s">
+        <v>186</v>
+      </c>
+      <c r="B34" t="s">
         <v>187</v>
       </c>
-      <c r="B34" t="s">
+      <c r="C34" t="s">
         <v>188</v>
       </c>
-      <c r="C34" t="s">
+      <c r="D34" t="s">
+        <v>179</v>
+      </c>
+      <c r="E34" t="s">
         <v>189</v>
       </c>
-      <c r="D34" t="s">
-        <v>180</v>
-      </c>
-      <c r="E34" t="s">
+      <c r="F34" t="s">
         <v>190</v>
-      </c>
-      <c r="F34" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A35" t="s">
+        <v>191</v>
+      </c>
+      <c r="B35" t="s">
         <v>192</v>
       </c>
-      <c r="B35" t="s">
+      <c r="C35" t="s">
         <v>193</v>
       </c>
-      <c r="C35" t="s">
-        <v>194</v>
-      </c>
       <c r="D35" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E35" t="s">
         <v>51</v>
       </c>
       <c r="F35" t="s">
+        <v>194</v>
+      </c>
+      <c r="G35" t="s">
         <v>195</v>
-      </c>
-      <c r="G35" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A36" t="s">
+        <v>196</v>
+      </c>
+      <c r="B36" t="s">
         <v>197</v>
       </c>
-      <c r="B36" t="s">
+      <c r="C36" t="s">
         <v>198</v>
       </c>
-      <c r="C36" t="s">
-        <v>199</v>
-      </c>
       <c r="D36" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E36" t="s">
         <v>63</v>
       </c>
       <c r="F36" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A37" t="s">
+        <v>200</v>
+      </c>
+      <c r="B37" t="s">
         <v>201</v>
       </c>
-      <c r="B37" t="s">
+      <c r="C37" t="s">
         <v>202</v>
       </c>
-      <c r="C37" t="s">
-        <v>203</v>
-      </c>
       <c r="D37" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E37" t="s">
         <v>18</v>
       </c>
       <c r="F37" t="s">
+        <v>203</v>
+      </c>
+      <c r="G37" t="s">
         <v>204</v>
-      </c>
-      <c r="G37" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A38" t="s">
+        <v>205</v>
+      </c>
+      <c r="B38" t="s">
         <v>206</v>
-      </c>
-      <c r="B38" t="s">
-        <v>207</v>
       </c>
       <c r="C38" t="s">
         <v>23</v>
@@ -2371,15 +2371,15 @@
         <v>24</v>
       </c>
       <c r="F38" t="s">
+        <v>207</v>
+      </c>
+      <c r="G38" t="s">
         <v>208</v>
-      </c>
-      <c r="G38" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A39" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B39" t="s">
         <v>33</v>
@@ -2402,7 +2402,7 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A40" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B40" t="s">
         <v>60</v>
@@ -2425,7 +2425,7 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A41" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B41" t="s">
         <v>22</v>
@@ -2448,7 +2448,7 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A42" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B42" t="s">
         <v>28</v>
@@ -2471,22 +2471,22 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A43" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B43" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="C43" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="D43" t="s">
         <v>62</v>
       </c>
       <c r="E43" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="F43" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="G43" t="s">
         <v>215</v>
@@ -2494,22 +2494,22 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A44" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B44" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="C44" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="D44" t="s">
         <v>62</v>
       </c>
       <c r="E44" t="s">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="F44" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="G44" t="s">
         <v>217</v>
@@ -2517,22 +2517,22 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A45" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B45" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="C45" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="D45" t="s">
         <v>62</v>
       </c>
       <c r="E45" t="s">
-        <v>18</v>
+        <v>51</v>
       </c>
       <c r="F45" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="G45" t="s">
         <v>219</v>
@@ -2540,68 +2540,51 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A46" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B46" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="C46" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="D46" t="s">
         <v>62</v>
       </c>
       <c r="E46" t="s">
-        <v>51</v>
+        <v>11</v>
       </c>
       <c r="F46" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="G46" t="s">
-        <v>221</v>
+        <v>58</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A47" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B47" t="s">
-        <v>55</v>
+        <v>233</v>
       </c>
       <c r="C47" t="s">
-        <v>56</v>
+        <v>229</v>
       </c>
       <c r="D47" t="s">
-        <v>62</v>
+        <v>230</v>
       </c>
       <c r="E47" t="s">
-        <v>11</v>
+        <v>51</v>
       </c>
       <c r="F47" t="s">
-        <v>57</v>
-      </c>
-      <c r="G47" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="B48" t="s">
-        <v>231</v>
-      </c>
-      <c r="C48" t="s">
-        <v>232</v>
-      </c>
-      <c r="D48" t="s">
-        <v>233</v>
-      </c>
-      <c r="E48" t="s">
-        <v>51</v>
+        <v>235</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:G1 B27:G27 A14:F18 A12:E12 G12 A13 B32:G32 A20:F21 A19:E19 B37:G47 B36:C36 E36:F36 B30:F30 A9:G11 A8:E8 G8 B35:G35 B34:F34 B33:F33 B22:F26 A3:G7 A2:F2 B28:F29" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:G1 B27:G27 A14:F18 A12 G12 A13 B32:G32 A20:F21 A19:E19 B37:G42 B36:C36 E36:F36 B30:F30 A9:G11 A8:E8 G8 B35:G35 B34:F34 B33:F33 B22:F26 A3:G7 A2:F2 B28:F29 B43:G46 C12:E12" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add data and fix current year
</commit_message>
<xml_diff>
--- a/data/DATA.xlsx
+++ b/data/DATA.xlsx
@@ -14,13 +14,30 @@
   <sheets>
     <sheet name="2026" sheetId="1" r:id="rId1"/>
     <sheet name="2025" sheetId="2" r:id="rId2"/>
+    <sheet name="2024" sheetId="3" r:id="rId3"/>
+    <sheet name="2023" sheetId="4" r:id="rId4"/>
+    <sheet name="2022" sheetId="5" r:id="rId5"/>
+    <sheet name="2021" sheetId="6" r:id="rId6"/>
+    <sheet name="2020" sheetId="7" r:id="rId7"/>
+    <sheet name="2019" sheetId="8" r:id="rId8"/>
+    <sheet name="2018" sheetId="9" r:id="rId9"/>
+    <sheet name="2017" sheetId="10" r:id="rId10"/>
+    <sheet name="2016" sheetId="11" r:id="rId11"/>
+    <sheet name="2015" sheetId="12" r:id="rId12"/>
+    <sheet name="2014" sheetId="13" r:id="rId13"/>
+    <sheet name="2013" sheetId="14" r:id="rId14"/>
+    <sheet name="2012" sheetId="15" r:id="rId15"/>
+    <sheet name="2011" sheetId="16" r:id="rId16"/>
+    <sheet name="2010" sheetId="17" r:id="rId17"/>
+    <sheet name="2009" sheetId="18" r:id="rId18"/>
+    <sheet name="2008" sheetId="19" r:id="rId19"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="243">
   <si>
     <t>id</t>
   </si>
@@ -728,7 +745,28 @@
     <t>Lê Văn Huy (Huy Lê)</t>
   </si>
   <si>
-    <t>Sâu sắc</t>
+    <t>Phan Đình Thành Nhân</t>
+  </si>
+  <si>
+    <t>Nhân</t>
+  </si>
+  <si>
+    <t>Cu em</t>
+  </si>
+  <si>
+    <t>Người anh sâu sắc</t>
+  </si>
+  <si>
+    <t>Lê Thị Minh Ngọc</t>
+  </si>
+  <si>
+    <t>Cá nọc</t>
+  </si>
+  <si>
+    <t>./images/LE_THI_MINH_NGOC.jpg</t>
+  </si>
+  <si>
+    <t>47</t>
   </si>
 </sst>
 </file>
@@ -1106,7 +1144,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
@@ -1514,7 +1552,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A18">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B18" t="s">
         <v>60</v>
@@ -1533,6 +1571,29 @@
       </c>
       <c r="G18" t="s">
         <v>65</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>239</v>
+      </c>
+      <c r="C19" t="s">
+        <v>76</v>
+      </c>
+      <c r="D19" t="s">
+        <v>62</v>
+      </c>
+      <c r="E19" t="s">
+        <v>63</v>
+      </c>
+      <c r="F19" t="s">
+        <v>240</v>
+      </c>
+      <c r="G19" t="s">
+        <v>241</v>
       </c>
     </row>
   </sheetData>
@@ -1543,12 +1604,134 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G47"/>
+  <dimension ref="A1:G48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="F48" sqref="F48"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -2578,7 +2761,30 @@
         <v>51</v>
       </c>
       <c r="F47" t="s">
-        <v>235</v>
+        <v>238</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A48" t="s">
+        <v>242</v>
+      </c>
+      <c r="B48" t="s">
+        <v>239</v>
+      </c>
+      <c r="C48" t="s">
+        <v>76</v>
+      </c>
+      <c r="D48" t="s">
+        <v>62</v>
+      </c>
+      <c r="E48" t="s">
+        <v>63</v>
+      </c>
+      <c r="F48" t="s">
+        <v>240</v>
+      </c>
+      <c r="G48" t="s">
+        <v>241</v>
       </c>
     </row>
   </sheetData>
@@ -2587,4 +2793,573 @@
     <ignoredError sqref="A1:G1 B27:G27 A14:F18 A12 G12 A13 B32:G32 A20:F21 A19:E19 B37:G42 B36:C36 E36:F36 B30:F30 A9:G11 A8:E8 G8 B35:G35 B34:F34 B33:F33 B22:F26 A3:G7 A2:F2 B28:F29 B43:G46 C12:E12" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <cols>
+    <col min="2" max="2" width="17.375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E3" t="s">
+        <v>72</v>
+      </c>
+      <c r="F3" t="s">
+        <v>73</v>
+      </c>
+      <c r="G3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="B4" t="s">
+        <v>233</v>
+      </c>
+      <c r="C4" t="s">
+        <v>229</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F4" t="s">
+        <v>238</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <cols>
+    <col min="2" max="2" width="19.5625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>197</v>
+      </c>
+      <c r="C2" t="s">
+        <v>198</v>
+      </c>
+      <c r="D2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F2" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>235</v>
+      </c>
+      <c r="C3" t="s">
+        <v>236</v>
+      </c>
+      <c r="D3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>233</v>
+      </c>
+      <c r="C4" t="s">
+        <v>229</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F4" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D6" t="s">
+        <v>174</v>
+      </c>
+      <c r="E6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" t="s">
+        <v>73</v>
+      </c>
+      <c r="G6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>197</v>
+      </c>
+      <c r="C2" t="s">
+        <v>198</v>
+      </c>
+      <c r="D2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F2" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>235</v>
+      </c>
+      <c r="C3" t="s">
+        <v>236</v>
+      </c>
+      <c r="D3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>197</v>
+      </c>
+      <c r="C2" t="s">
+        <v>198</v>
+      </c>
+      <c r="D2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F2" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>235</v>
+      </c>
+      <c r="C3" t="s">
+        <v>236</v>
+      </c>
+      <c r="D3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>197</v>
+      </c>
+      <c r="C2" t="s">
+        <v>198</v>
+      </c>
+      <c r="D2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F2" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>235</v>
+      </c>
+      <c r="C3" t="s">
+        <v>236</v>
+      </c>
+      <c r="D3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>197</v>
+      </c>
+      <c r="C2" t="s">
+        <v>198</v>
+      </c>
+      <c r="D2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F2" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>235</v>
+      </c>
+      <c r="C3" t="s">
+        <v>236</v>
+      </c>
+      <c r="D3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>